<commit_message>
Update MT_OntoWorldMap_2023-06-13.xlsx with RXNO, BAO, MOP
</commit_message>
<xml_diff>
--- a/master_table/MT_OntoWorldMap_2023-06-13.xlsx
+++ b/master_table/MT_OntoWorldMap_2023-06-13.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="19" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Template mit Beispiel" sheetId="4" r:id="rId1"/>
@@ -34,10 +34,12 @@
     <sheet name="PIMS-II" sheetId="20" r:id="rId20"/>
     <sheet name="EDAM" sheetId="21" r:id="rId21"/>
     <sheet name="RXNO" sheetId="22" r:id="rId22"/>
+    <sheet name="MOP" sheetId="23" r:id="rId23"/>
+    <sheet name="BAO" sheetId="25" r:id="rId24"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">BFO!$A$1:$A$93</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">List_zu_betrachtende_Ontologien!$A$1:$J$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">List_zu_betrachtende_Ontologien!$A$1:$J$35</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -60,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2096" uniqueCount="489">
   <si>
     <t>Ontology</t>
   </si>
@@ -814,9 +816,6 @@
   </si>
   <si>
     <t>non inferred</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC-BY-4.0 license </t>
   </si>
   <si>
     <t>25ms</t>
@@ -1271,9 +1270,6 @@
     <t>unknown</t>
   </si>
   <si>
-    <t>CC-BY-4.0 license ? The emmo repo is cc-by-4 the subrepo which should have its own licence has none attached</t>
-  </si>
-  <si>
     <t>http://emmo.info/domain-crystallography/cif_top</t>
   </si>
   <si>
@@ -1472,9 +1468,6 @@
     <t>RXNO: name reaction ontology</t>
   </si>
   <si>
-    <t>CC-BY-4.0 license</t>
-  </si>
-  <si>
     <t>https://en.wikipedia.org/wiki/RXNO_Ontology</t>
   </si>
   <si>
@@ -1514,10 +1507,76 @@
     <t>chebi,dc,obo,oboInOwl,owl,rdf,rdfs,terms,xml,xsd</t>
   </si>
   <si>
-    <t>rdfs:label, IAO_0000115 for definitions</t>
-  </si>
-  <si>
-    <t>It contains more than 500 classes representing organic reactions such as the Diels–Alder cyclization. The documentation also contains a good overview on how to reuse the classes contained in this ontology.</t>
+    <t>MOP</t>
+  </si>
+  <si>
+    <t>molecular process ontology</t>
+  </si>
+  <si>
+    <t>Molecular Process Ontology</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/rsc-ontologies/rxno/master/mop.owl</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Strongly connected with the RXNO. It contains the underlying molecular processes, for example cyclization, methylation and demethylation.</t>
+  </si>
+  <si>
+    <t>Strongly connected with the MOP. It contains more than 500 classes representing organic reactions such as the Diels–Alder cyclization. The documentation also contains a good overview on how to reuse the classes contained in this ontology.</t>
+  </si>
+  <si>
+    <t>172 ms</t>
+  </si>
+  <si>
+    <t>dc,mop,obo,oboInOwl,owl,rdf,rdfs,terms,xml,xsd</t>
+  </si>
+  <si>
+    <t>http://bioassayontology.org/</t>
+  </si>
+  <si>
+    <t>doi:10.1186/2041-1480-5-S1-S5 ; doi:10.1371/journal.pone.0049198  ; doi:10.1186/1471-2105-12-257</t>
+  </si>
+  <si>
+    <t>https://github.com/BioAssayOntology</t>
+  </si>
+  <si>
+    <t>CC-BY-4.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC-BY-4.0 </t>
+  </si>
+  <si>
+    <t>CC-BY-4.0 ? The emmo repo is cc-by-4 the subrepo which should have its own licence has none attached</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/BioAssayOntology/BAO/master/bao_complete_merged.owl</t>
+  </si>
+  <si>
+    <t>Describes chemical biology screening assays and their results including high-throughput screening (HTS) data for the purpose of categorizing assays and data analysis.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quite applied and in active development, see also here: http://bioassayontology.org/bao-bioportal/ </t>
+  </si>
+  <si>
+    <t>Hande Küçük McGinty, Janice Kranz, Joseph Ostrow, Alex Clark, Yu Lin, Saminda Abeyruwan, Uma Vempati, Kunie Sakurai, Vance Lemmon, Ubbo Visser, John Turner, Nicolette Ross, Joan Glenny-Pescov, Jiaming Hu, Caty Chung, Stephan Schurer*</t>
+  </si>
+  <si>
+    <t>University of Miami, Ontology is still actively maintained</t>
+  </si>
+  <si>
+    <t>bao,bao1,cellline,core,dc,efo,foaf,obo,oboInOwl,owl,protege,rdf,rdfs,skos,xml,xsd</t>
+  </si>
+  <si>
+    <t>non inferred, available as merged version</t>
+  </si>
+  <si>
+    <t>215 ms</t>
+  </si>
+  <si>
+    <t>rdfs:label, OBO:IAO_0000115 for textual definitions</t>
+  </si>
+  <si>
+    <t>related:narrower</t>
   </si>
 </sst>
 </file>
@@ -1879,7 +1938,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2038,6 +2097,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2456,7 +2521,7 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
@@ -2883,7 +2948,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -2893,7 +2958,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -2903,7 +2968,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -2913,7 +2978,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -2928,7 +2993,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -2938,7 +3003,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -2948,7 +3013,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="60" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -2958,17 +3023,17 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="40" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -2978,12 +3043,12 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
@@ -2993,7 +3058,7 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
@@ -3003,7 +3068,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
@@ -3013,7 +3078,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
@@ -3023,7 +3088,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
@@ -3033,7 +3098,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
@@ -3043,7 +3108,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
@@ -3053,7 +3118,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
@@ -3063,7 +3128,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -3298,7 +3363,7 @@
     </row>
     <row r="94" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="35" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
@@ -3349,7 +3414,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -3369,7 +3434,7 @@
     </row>
     <row r="9" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -3379,7 +3444,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3394,7 +3459,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -3404,7 +3469,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -3414,7 +3479,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -3424,17 +3489,17 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3444,12 +3509,12 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
@@ -3459,7 +3524,7 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
@@ -3469,7 +3534,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
@@ -3479,7 +3544,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
@@ -3489,7 +3554,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
@@ -3499,7 +3564,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
@@ -3509,7 +3574,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
@@ -3519,7 +3584,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
@@ -3529,7 +3594,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3764,7 +3829,7 @@
     </row>
     <row r="94" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="35" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
@@ -3809,7 +3874,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -3839,7 +3904,7 @@
     </row>
     <row r="9" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="40" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -3849,7 +3914,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3864,7 +3929,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -3874,7 +3939,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -3894,17 +3959,17 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3914,12 +3979,12 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
@@ -3939,7 +4004,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
@@ -3949,7 +4014,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
@@ -3969,7 +4034,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
@@ -3979,7 +4044,7 @@
     </row>
     <row r="39" spans="1:1" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
@@ -3989,7 +4054,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
@@ -3999,7 +4064,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4234,12 +4299,12 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="38" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
@@ -4296,7 +4361,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -4381,12 +4446,12 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
@@ -4401,12 +4466,12 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
@@ -4426,7 +4491,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
@@ -4436,7 +4501,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
@@ -4446,7 +4511,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
@@ -4456,7 +4521,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
@@ -4466,7 +4531,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
@@ -4476,7 +4541,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
@@ -4486,7 +4551,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -4621,7 +4686,7 @@
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
@@ -4721,7 +4786,7 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="38" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
@@ -4804,7 +4869,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="63" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -4814,7 +4879,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -4829,7 +4894,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -4839,7 +4904,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="21" x14ac:dyDescent="0.3">
@@ -4860,17 +4925,17 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -4880,7 +4945,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -4905,7 +4970,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -4915,7 +4980,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
@@ -4925,7 +4990,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
@@ -4935,7 +5000,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
@@ -4945,7 +5010,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
@@ -4955,7 +5020,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
@@ -4965,7 +5030,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -5100,7 +5165,7 @@
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
@@ -5200,7 +5265,7 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="38" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
@@ -5254,7 +5319,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -5284,7 +5349,7 @@
     </row>
     <row r="9" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A9" s="40" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -5294,7 +5359,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
@@ -5309,7 +5374,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -5319,7 +5384,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -5329,7 +5394,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -5339,17 +5404,17 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
@@ -5359,12 +5424,12 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
@@ -5374,7 +5439,7 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
@@ -5384,7 +5449,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
@@ -5394,7 +5459,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
@@ -5414,7 +5479,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
@@ -5424,7 +5489,7 @@
     </row>
     <row r="39" spans="1:1" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
@@ -5434,7 +5499,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
@@ -5444,7 +5509,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
@@ -5679,7 +5744,7 @@
     </row>
     <row r="93" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A93" s="38" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
@@ -5716,7 +5781,7 @@
   <dimension ref="A1:D126"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5737,7 +5802,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.3">
@@ -5747,7 +5812,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.3">
@@ -5757,7 +5822,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.3">
@@ -5803,7 +5868,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="71" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C17" s="71"/>
     </row>
@@ -5829,7 +5894,7 @@
     </row>
     <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -5844,12 +5909,12 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -5859,7 +5924,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -5869,7 +5934,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="71" t="s">
-        <v>387</v>
+        <v>478</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -5889,7 +5954,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
@@ -5909,7 +5974,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
@@ -5929,7 +5994,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -6164,7 +6229,7 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="39" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
@@ -6228,7 +6293,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -6238,7 +6303,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -6248,7 +6313,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="71" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -6273,7 +6338,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -6283,7 +6348,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -6293,7 +6358,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -6303,17 +6368,17 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="71" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -6323,7 +6388,7 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
@@ -6348,7 +6413,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
@@ -6378,7 +6443,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
@@ -6388,7 +6453,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
@@ -6398,7 +6463,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
@@ -6408,7 +6473,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -6643,7 +6708,7 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="39" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
@@ -6697,7 +6762,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -6727,7 +6792,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -6737,7 +6802,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -6752,7 +6817,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -6762,7 +6827,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -6772,7 +6837,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -6787,12 +6852,12 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="71" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -6802,12 +6867,12 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
@@ -6817,7 +6882,7 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
@@ -6827,7 +6892,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
@@ -6847,7 +6912,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="39" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
@@ -6857,7 +6922,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
@@ -6867,7 +6932,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
@@ -6887,7 +6952,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -7122,7 +7187,7 @@
     </row>
     <row r="93" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="72" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
@@ -7175,7 +7240,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -7205,7 +7270,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -7215,7 +7280,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -7230,7 +7295,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -7240,7 +7305,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -7265,7 +7330,7 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
@@ -7280,12 +7345,12 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
@@ -7295,7 +7360,7 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
@@ -7325,7 +7390,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="39" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
@@ -7335,7 +7400,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
@@ -7345,7 +7410,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
@@ -7600,7 +7665,7 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="72" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
@@ -7626,12 +7691,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:AU34"/>
+  <dimension ref="A1:AU35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="71.88671875" defaultRowHeight="69.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7680,7 +7744,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
         <v>92</v>
       </c>
@@ -7712,7 +7776,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
         <v>101</v>
       </c>
@@ -7776,7 +7840,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
         <v>114</v>
       </c>
@@ -7808,7 +7872,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="61" t="s">
         <v>119</v>
       </c>
@@ -7840,7 +7904,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="34" t="s">
         <v>6</v>
       </c>
@@ -7904,7 +7968,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34" t="s">
         <v>136</v>
       </c>
@@ -7968,7 +8032,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="34" t="s">
         <v>148</v>
       </c>
@@ -7998,7 +8062,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="34" t="s">
         <v>154</v>
       </c>
@@ -8058,7 +8122,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="59" t="s">
         <v>166</v>
       </c>
@@ -8116,7 +8180,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="59" t="s">
         <v>179</v>
       </c>
@@ -8144,7 +8208,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="17" spans="1:47" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:47" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="58" t="s">
         <v>185</v>
       </c>
@@ -8204,250 +8268,256 @@
         <v>194</v>
       </c>
     </row>
-    <row r="19" spans="1:47" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="34" t="s">
+    <row r="19" spans="1:47" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="77" t="s">
+        <v>465</v>
+      </c>
+      <c r="B19" s="78"/>
+      <c r="C19" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" t="s">
+        <v>466</v>
+      </c>
+      <c r="E19" s="21"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="22"/>
+    </row>
+    <row r="20" spans="1:47" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="34" t="s">
         <v>195</v>
       </c>
-      <c r="B19" s="65" t="s">
+      <c r="B20" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C20" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D20" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="16" t="s">
+      <c r="E20" s="21"/>
+      <c r="F20" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G20" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H20" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="I19" s="16" t="s">
+      <c r="I20" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="J19" s="16" t="s">
+      <c r="J20" s="16" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="20" spans="1:47" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="58" t="s">
+    <row r="21" spans="1:47" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="B20" s="68" t="s">
+      <c r="B21" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C21" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="D21" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E21" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="F20" s="29" t="s">
+      <c r="F21" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="G20" s="30" t="s">
+      <c r="G21" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="H20" s="30" t="s">
+      <c r="H21" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="I20" s="28" t="s">
+      <c r="I21" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="J20" s="27" t="s">
+      <c r="J21" s="27" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:47" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="34" t="s">
+    <row r="22" spans="1:47" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="B21" s="65" t="s">
+      <c r="B22" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="H21" s="31"/>
-      <c r="I21" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="J21" s="16" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="22" spans="1:47" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="B22" s="22"/>
       <c r="C22" s="22" t="s">
         <v>109</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E22" s="21"/>
       <c r="F22" s="21"/>
-      <c r="G22" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="H22" s="16" t="s">
-        <v>211</v>
-      </c>
+      <c r="G22" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="H22" s="31"/>
       <c r="I22" s="16" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:47" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="B23" s="22"/>
+      <c r="A23" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>93</v>
+      </c>
       <c r="C23" s="22" t="s">
         <v>109</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E23" s="21"/>
       <c r="F23" s="21"/>
-      <c r="G23" s="16" t="s">
+      <c r="G23" s="71" t="s">
+        <v>210</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="1:47" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="H23" s="16" t="s">
+      <c r="H24" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="I23" s="16" t="s">
+      <c r="I24" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="J23" s="16" t="s">
+      <c r="J24" s="16" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:47" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="34" t="s">
+    <row r="25" spans="1:47" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="34" t="s">
         <v>220</v>
-      </c>
-      <c r="B24" s="65" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="G24" s="71" t="s">
-        <v>222</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="I24" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="J24" s="16" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="25" spans="1:47" s="32" customFormat="1" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="34" t="s">
-        <v>226</v>
       </c>
       <c r="B25" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="D25" t="s">
-        <v>227</v>
-      </c>
-      <c r="E25"/>
-      <c r="F25"/>
-      <c r="G25"/>
-      <c r="H25"/>
-      <c r="I25"/>
-      <c r="J25"/>
-      <c r="K25"/>
-      <c r="L25"/>
-      <c r="M25"/>
-      <c r="N25"/>
-      <c r="O25"/>
-      <c r="P25"/>
-      <c r="Q25"/>
-      <c r="R25"/>
-      <c r="S25"/>
-      <c r="T25"/>
-      <c r="U25"/>
-      <c r="V25"/>
-      <c r="W25"/>
-      <c r="X25"/>
-      <c r="Y25"/>
-      <c r="Z25"/>
-      <c r="AA25"/>
-      <c r="AB25"/>
-      <c r="AC25"/>
-      <c r="AD25"/>
-      <c r="AE25"/>
-      <c r="AF25"/>
-      <c r="AG25"/>
-      <c r="AH25"/>
-      <c r="AI25"/>
-      <c r="AJ25"/>
-      <c r="AK25"/>
-      <c r="AL25"/>
-      <c r="AM25"/>
-      <c r="AN25"/>
-      <c r="AO25"/>
-      <c r="AP25"/>
-      <c r="AQ25"/>
-      <c r="AR25"/>
-      <c r="AS25"/>
-      <c r="AT25"/>
-      <c r="AU25"/>
-    </row>
-    <row r="26" spans="1:47" s="32" customFormat="1" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="E25" s="21"/>
+      <c r="F25" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="G25" s="71" t="s">
+        <v>222</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:47" s="32" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="34" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B26" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="32" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="27" spans="1:47" s="32" customFormat="1" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>227</v>
+      </c>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+      <c r="P26"/>
+      <c r="Q26"/>
+      <c r="R26"/>
+      <c r="S26"/>
+      <c r="T26"/>
+      <c r="U26"/>
+      <c r="V26"/>
+      <c r="W26"/>
+      <c r="X26"/>
+      <c r="Y26"/>
+      <c r="Z26"/>
+      <c r="AA26"/>
+      <c r="AB26"/>
+      <c r="AC26"/>
+      <c r="AD26"/>
+      <c r="AE26"/>
+      <c r="AF26"/>
+      <c r="AG26"/>
+      <c r="AH26"/>
+      <c r="AI26"/>
+      <c r="AJ26"/>
+      <c r="AK26"/>
+      <c r="AL26"/>
+      <c r="AM26"/>
+      <c r="AN26"/>
+      <c r="AO26"/>
+      <c r="AP26"/>
+      <c r="AQ26"/>
+      <c r="AR26"/>
+      <c r="AS26"/>
+      <c r="AT26"/>
+      <c r="AU26"/>
+    </row>
+    <row r="27" spans="1:47" s="32" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="34" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B27" s="65" t="s">
         <v>93</v>
@@ -8456,83 +8526,91 @@
         <v>102</v>
       </c>
       <c r="D27" s="32" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="28" spans="1:47" s="32" customFormat="1" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="59" t="s">
-        <v>232</v>
-      </c>
-      <c r="B28" s="67" t="s">
-        <v>120</v>
+        <v>229</v>
+      </c>
+    </row>
+    <row r="28" spans="1:47" s="32" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="B28" s="65" t="s">
+        <v>93</v>
       </c>
       <c r="C28" s="32" t="s">
         <v>102</v>
       </c>
       <c r="D28" s="32" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="29" spans="1:47" s="32" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="59" t="s">
+        <v>232</v>
+      </c>
+      <c r="B29" s="67" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="32" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="29" spans="1:47" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="30" spans="1:47" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>234</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:47" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="73" t="s">
-        <v>442</v>
-      </c>
-      <c r="C30" s="32" t="s">
+    <row r="31" spans="1:47" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="73" t="s">
+        <v>440</v>
+      </c>
+      <c r="C31" s="32" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:47" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>235</v>
-      </c>
-      <c r="B31">
-        <f>COUNTA(A2:A29)</f>
-        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:47" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B32">
-        <f>COUNTA(B2:B29)</f>
-        <v>25</v>
+        <f>COUNTA(A2:A30)</f>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B33">
-        <f>COUNTIF(B2:B29,"x")</f>
-        <v>18</v>
+        <f>COUNTA(B2:B30)</f>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>237</v>
+      </c>
+      <c r="B34">
+        <f>COUNTIF(B2:B30,"x")</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>238</v>
       </c>
-      <c r="B34">
-        <f>B32/B31*100</f>
-        <v>89.285714285714292</v>
+      <c r="B35">
+        <f>B33/B32*100</f>
+        <v>89.65517241379311</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J34">
-    <filterColumn colId="2">
-      <filters blank="1">
-        <filter val="be"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J35"/>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
     <hyperlink ref="H2" r:id="rId2"/>
@@ -8560,13 +8638,14 @@
     <hyperlink ref="G17" r:id="rId24" location=".YYVO9LoxlPY"/>
     <hyperlink ref="H17" r:id="rId25"/>
     <hyperlink ref="H18" r:id="rId26"/>
-    <hyperlink ref="H19" r:id="rId27"/>
-    <hyperlink ref="G20" r:id="rId28"/>
-    <hyperlink ref="H20" r:id="rId29"/>
-    <hyperlink ref="G21" r:id="rId30"/>
-    <hyperlink ref="G19" r:id="rId31"/>
+    <hyperlink ref="H20" r:id="rId27"/>
+    <hyperlink ref="G21" r:id="rId28"/>
+    <hyperlink ref="H21" r:id="rId29"/>
+    <hyperlink ref="G22" r:id="rId30"/>
+    <hyperlink ref="G20" r:id="rId31"/>
     <hyperlink ref="G18" r:id="rId32"/>
-    <hyperlink ref="G24" r:id="rId33"/>
+    <hyperlink ref="G25" r:id="rId33"/>
+    <hyperlink ref="G23" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8628,7 +8707,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -8638,7 +8717,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -8653,7 +8732,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -8663,7 +8742,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -8688,12 +8767,12 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="71" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -8703,12 +8782,12 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
@@ -8718,7 +8797,7 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
@@ -8728,7 +8807,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="71" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
@@ -8738,7 +8817,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
@@ -8748,7 +8827,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="39" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
@@ -8758,7 +8837,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
@@ -8768,7 +8847,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
@@ -8788,7 +8867,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -9018,7 +9097,7 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="72" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
@@ -9049,7 +9128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A126"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -9071,7 +9150,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -9101,7 +9180,7 @@
     </row>
     <row r="9" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -9111,7 +9190,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -9126,7 +9205,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="71" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -9136,7 +9215,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -9146,7 +9225,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -9156,17 +9235,17 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="71" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -9176,12 +9255,12 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
@@ -9191,7 +9270,7 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
@@ -9201,7 +9280,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="71" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
@@ -9211,7 +9290,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
@@ -9221,7 +9300,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="39" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
@@ -9231,7 +9310,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
@@ -9241,7 +9320,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
@@ -9261,7 +9340,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -9491,7 +9570,7 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="72" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
@@ -9524,8 +9603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A93"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9545,7 +9624,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -9575,7 +9654,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -9585,7 +9664,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -9621,7 +9700,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="71" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -9636,12 +9715,12 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="71" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -9652,7 +9731,7 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
@@ -9665,6 +9744,11 @@
         <v>23</v>
       </c>
     </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>246</v>
+      </c>
+    </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>25</v>
@@ -9672,7 +9756,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="74" t="s">
-        <v>454</v>
+        <v>476</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
@@ -9682,7 +9766,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="75" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
@@ -9692,7 +9776,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="39" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
@@ -9702,7 +9786,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="76" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
@@ -9722,7 +9806,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="39" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
@@ -9732,7 +9816,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="39" t="s">
-        <v>468</v>
+        <v>487</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -9965,7 +10049,930 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
+        <v>470</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A93"/>
+  <sheetViews>
+    <sheetView topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="143.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="71" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="71" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="71" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="71" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="71" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="74" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="75" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="39" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="76" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="39" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="39" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="39" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="45" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="74" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A75" s="37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" s="38">
+        <v>22843</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A77" s="37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" s="39">
+        <v>3819</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A79" s="37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" s="39">
+        <v>3724</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A81" s="37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="39">
+        <v>3686</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A83" s="37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="39">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A85" s="37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A87" s="37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A89" s="37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" s="39">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="92" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>469</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A94"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="143.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="71" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="71" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="71" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="71" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="74" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="75" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="39" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="76" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="39" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="39" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="39" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="45" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="74" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A75" s="37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" s="38">
+        <v>92149</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A77" s="37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" s="39">
+        <v>10052</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A79" s="37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" s="39">
+        <v>7838</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A81" s="37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="39">
+        <v>7512</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A83" s="37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="39">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A85" s="37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="39">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A87" s="37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A89" s="37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" s="39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="92" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -10091,7 +11098,7 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
@@ -10107,7 +11114,7 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
@@ -10457,7 +11464,7 @@
   <dimension ref="A1:A95"/>
   <sheetViews>
     <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10567,7 +11574,7 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
@@ -10582,7 +11589,7 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
@@ -10607,7 +11614,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>247</v>
+        <v>477</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
@@ -10617,7 +11624,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
@@ -10627,7 +11634,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
@@ -10637,7 +11644,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
@@ -10657,7 +11664,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
@@ -10667,7 +11674,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
@@ -10897,17 +11904,17 @@
     </row>
     <row r="93" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A93" s="38" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" s="41" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" s="41" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -10948,7 +11955,7 @@
     </row>
     <row r="3" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10978,7 +11985,7 @@
     </row>
     <row r="9" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10988,7 +11995,7 @@
     </row>
     <row r="11" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11003,7 +12010,7 @@
     </row>
     <row r="15" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11013,7 +12020,7 @@
     </row>
     <row r="17" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11023,7 +12030,7 @@
     </row>
     <row r="19" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11033,17 +12040,17 @@
     </row>
     <row r="21" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11053,12 +12060,12 @@
     </row>
     <row r="26" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11078,7 +12085,7 @@
     </row>
     <row r="31" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11108,7 +12115,7 @@
     </row>
     <row r="37" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11118,7 +12125,7 @@
     </row>
     <row r="39" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11273,7 +12280,7 @@
     </row>
     <row r="71" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11368,7 +12375,7 @@
     </row>
     <row r="93" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -11438,7 +12445,7 @@
     </row>
     <row r="9" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A9" s="40" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.4">
@@ -11448,7 +12455,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
@@ -11486,7 +12493,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="21" x14ac:dyDescent="0.4">
@@ -11496,17 +12503,17 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
@@ -11519,12 +12526,12 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="50" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
@@ -11534,7 +12541,7 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
@@ -11544,7 +12551,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
@@ -11554,7 +12561,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="16" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
@@ -11564,7 +12571,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
@@ -11574,7 +12581,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
@@ -11584,7 +12591,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="22" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
@@ -11594,7 +12601,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
@@ -11604,7 +12611,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
@@ -11846,7 +12853,7 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
@@ -11917,7 +12924,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -11952,7 +12959,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -11977,12 +12984,12 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
@@ -11992,12 +12999,12 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
@@ -12007,7 +13014,7 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
@@ -12017,7 +13024,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
@@ -12027,7 +13034,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
@@ -12047,7 +13054,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
@@ -12057,7 +13064,7 @@
     </row>
     <row r="39" spans="1:1" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
@@ -12067,7 +13074,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
@@ -12077,7 +13084,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
@@ -12312,7 +13319,7 @@
     </row>
     <row r="93" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A93" s="38" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
@@ -12368,7 +13375,7 @@
     </row>
     <row r="3" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12378,7 +13385,7 @@
     </row>
     <row r="5" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12398,7 +13405,7 @@
     </row>
     <row r="9" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12408,7 +13415,7 @@
     </row>
     <row r="11" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -12423,7 +13430,7 @@
     </row>
     <row r="15" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12433,7 +13440,7 @@
     </row>
     <row r="17" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12458,12 +13465,12 @@
     </row>
     <row r="22" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -12473,12 +13480,12 @@
     </row>
     <row r="26" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12488,7 +13495,7 @@
     </row>
     <row r="29" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12498,7 +13505,7 @@
     </row>
     <row r="31" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12508,7 +13515,7 @@
     </row>
     <row r="33" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12518,7 +13525,7 @@
     </row>
     <row r="35" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12528,7 +13535,7 @@
     </row>
     <row r="37" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12538,7 +13545,7 @@
     </row>
     <row r="39" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12548,7 +13555,7 @@
     </row>
     <row r="41" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12558,7 +13565,7 @@
     </row>
     <row r="43" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -12693,7 +13700,7 @@
     </row>
     <row r="71" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12793,7 +13800,7 @@
     </row>
     <row r="93" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -12827,7 +13834,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -12857,7 +13864,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -12867,7 +13874,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
@@ -12892,7 +13899,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -12917,7 +13924,7 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
@@ -12932,12 +13939,12 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
@@ -12947,7 +13954,7 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
@@ -12957,7 +13964,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
@@ -12967,7 +13974,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
@@ -12977,7 +13984,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
@@ -12987,7 +13994,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
@@ -12997,7 +14004,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
@@ -13007,7 +14014,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
@@ -13017,7 +14024,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
@@ -13252,7 +14259,7 @@
     </row>
     <row r="94" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="35" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Collection close to complete
</commit_message>
<xml_diff>
--- a/master_table/MT_OntoWorldMap_2023-06-13.xlsx
+++ b/master_table/MT_OntoWorldMap_2023-06-13.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2287" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2289" uniqueCount="529">
   <si>
     <t>Ontology</t>
   </si>
@@ -11623,8 +11623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -11833,7 +11833,9 @@
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="74"/>
+      <c r="A33" s="74" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="3" t="s">
@@ -11841,7 +11843,9 @@
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="38"/>
+      <c r="A35" s="38" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="3" t="s">

</xml_diff>